<commit_message>
-Quito las islas -Ajusto las proporciones de los labels de los botones para que todos esten al mismo tamaño de fuente. -->Falta ajustar los textos diagonales -Renombro los videos de CHICCO y SWAROVSKI de modo que coincidan con los nombres de sus respectivos botones y puedan ser cargados por EasyMovieTexture.
</commit_message>
<xml_diff>
--- a/MapaOutlet/Assets/References/Directorio locales.xlsx
+++ b/MapaOutlet/Assets/References/Directorio locales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="439">
   <si>
     <t>DIRECTORIO OUTLET PUEBLA</t>
   </si>
@@ -481,9 +481,6 @@
   </si>
   <si>
     <t>HUGO PICHARDO</t>
-  </si>
-  <si>
-    <t>DIRECTORIO OUTLET PREMIER</t>
   </si>
   <si>
     <t>A-9</t>
@@ -920,6 +917,474 @@
   </si>
   <si>
     <t>PRIMERAS 30</t>
+  </si>
+  <si>
+    <t>VANS+O-1#2105899</t>
+  </si>
+  <si>
+    <t>WILSON+O-2A#2221173328</t>
+  </si>
+  <si>
+    <t>SPRINGFIELD+O-2B#6885801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GILLIO+O-3A#2106589/2106661 </t>
+  </si>
+  <si>
+    <t>TRUE RELIGION+O-4#2319946</t>
+  </si>
+  <si>
+    <t>BRANTANO+O-5</t>
+  </si>
+  <si>
+    <t>NINE WEST+O-6</t>
+  </si>
+  <si>
+    <t>FLEXI+Q-1</t>
+  </si>
+  <si>
+    <t>REDUCED+Q-2</t>
+  </si>
+  <si>
+    <t>CHIQUIMUNDO+A-5</t>
+  </si>
+  <si>
+    <t>SALOMON+P-1</t>
+  </si>
+  <si>
+    <t>BENETTON+P-2</t>
+  </si>
+  <si>
+    <t>SAVI JEANS+P-3A</t>
+  </si>
+  <si>
+    <t>CROCS+P-3B</t>
+  </si>
+  <si>
+    <t>CAPA DE OZONO+P-4</t>
+  </si>
+  <si>
+    <t>FERRAGAMO+P-5</t>
+  </si>
+  <si>
+    <t>SKECHERS+Q-3</t>
+  </si>
+  <si>
+    <t>NIKE+V-1</t>
+  </si>
+  <si>
+    <t>ADOLFO DOMINGUEZ+P-6</t>
+  </si>
+  <si>
+    <t>SWAROVSKI+Q-4A</t>
+  </si>
+  <si>
+    <t>JULIO+P-7</t>
+  </si>
+  <si>
+    <t>HUGO BOSS+Q-4B</t>
+  </si>
+  <si>
+    <t>CARTER'S OSHKOSH+Q-5</t>
+  </si>
+  <si>
+    <t>IVONNE+Q-6</t>
+  </si>
+  <si>
+    <t>TIMEOUT+A-4A</t>
+  </si>
+  <si>
+    <t>SHOWSPORT+A-4B</t>
+  </si>
+  <si>
+    <t>SILVER PLATE+A-3</t>
+  </si>
+  <si>
+    <t>ARENA+A-2</t>
+  </si>
+  <si>
+    <t>TED KENTON+D-1</t>
+  </si>
+  <si>
+    <t>FUROR+H-1</t>
+  </si>
+  <si>
+    <t>MARSEL+H-2</t>
+  </si>
+  <si>
+    <t>VIA URBANA+H-4</t>
+  </si>
+  <si>
+    <t>LIZ MINELLI+H-4A</t>
+  </si>
+  <si>
+    <t>SAMSONITE+H-4B</t>
+  </si>
+  <si>
+    <t>UNDER ARMOUR+U-2</t>
+  </si>
+  <si>
+    <t>STUDIO F+U-1</t>
+  </si>
+  <si>
+    <t>GUESS+R-1</t>
+  </si>
+  <si>
+    <t>ROBERT'S+Q-7</t>
+  </si>
+  <si>
+    <t>JESSY FRANZ+A-5A</t>
+  </si>
+  <si>
+    <t>BORSETTA+A-6</t>
+  </si>
+  <si>
+    <t>TENNIS OFF+B-1-2</t>
+  </si>
+  <si>
+    <t>MABEL+B-5</t>
+  </si>
+  <si>
+    <t>CHICCO+B-6</t>
+  </si>
+  <si>
+    <t>LEVI'S+D-2</t>
+  </si>
+  <si>
+    <t>ROCKPORT+I-2</t>
+  </si>
+  <si>
+    <t>ASICS+I-4</t>
+  </si>
+  <si>
+    <t>CALVIN KLEIN+K-8</t>
+  </si>
+  <si>
+    <t>VANITY+M-1</t>
+  </si>
+  <si>
+    <t>CLOE+R-1</t>
+  </si>
+  <si>
+    <t>REWIND+Q-8</t>
+  </si>
+  <si>
+    <t>JUGUETRON+A-7</t>
+  </si>
+  <si>
+    <t>PRADA+R-3A</t>
+  </si>
+  <si>
+    <t>BCBG+Q-9</t>
+  </si>
+  <si>
+    <t>SUNGLASS HUT+R-3B</t>
+  </si>
+  <si>
+    <t>MANGO+Q-10</t>
+  </si>
+  <si>
+    <t>FASHION BABY+B-4, B-7</t>
+  </si>
+  <si>
+    <t>CHARLY+D-7</t>
+  </si>
+  <si>
+    <t>FERRIONI+D-4</t>
+  </si>
+  <si>
+    <t>MEN'S FACTORY+I-5</t>
+  </si>
+  <si>
+    <t>VICKY FORM+I-3</t>
+  </si>
+  <si>
+    <t>CELIO+I-6</t>
+  </si>
+  <si>
+    <t>OUTLET DEPORTES 01+M-2</t>
+  </si>
+  <si>
+    <t>LACOSTE+R-4</t>
+  </si>
+  <si>
+    <t>NUTRISSA+F-1</t>
+  </si>
+  <si>
+    <t>LA CAMISERIA PREMIER+J-8</t>
+  </si>
+  <si>
+    <t>CHILDREN'S SHOES+C-1-2</t>
+  </si>
+  <si>
+    <t>VITTORIO FORTI+C-5</t>
+  </si>
+  <si>
+    <t>DAVID SERRANO+E-1</t>
+  </si>
+  <si>
+    <t>VANITY+E-5</t>
+  </si>
+  <si>
+    <t>STYLO+J-1</t>
+  </si>
+  <si>
+    <t>CAVALIER+J-4</t>
+  </si>
+  <si>
+    <t>PEPE JEANS+L-1</t>
+  </si>
+  <si>
+    <t>VERTICHE+L-2-4</t>
+  </si>
+  <si>
+    <t>REDUCED+L-5</t>
+  </si>
+  <si>
+    <t>FRESH &amp; CREPES+F-2</t>
+  </si>
+  <si>
+    <t>PARFUMS RACHELLE+C-6</t>
+  </si>
+  <si>
+    <t>ZN ZAPATERIAS+E-2</t>
+  </si>
+  <si>
+    <t>URBAN STORE+J-2</t>
+  </si>
+  <si>
+    <t>BROOKS BROTHERS+L-3</t>
+  </si>
+  <si>
+    <t>7 CHILES+F-3</t>
+  </si>
+  <si>
+    <t>VIA CORTA+C-3</t>
+  </si>
+  <si>
+    <t>ZWILLING J.A. HENCKLES+C-7A</t>
+  </si>
+  <si>
+    <t>GEORGIE BOY+E-3</t>
+  </si>
+  <si>
+    <t>OGGI JEANS+E-7</t>
+  </si>
+  <si>
+    <t>TOMMY HILFIGER+N-6</t>
+  </si>
+  <si>
+    <t>BBVA BANCOMER+N-5</t>
+  </si>
+  <si>
+    <t>ITALIAN COFFEE+F-14</t>
+  </si>
+  <si>
+    <t>SHIRUSHI+F-13</t>
+  </si>
+  <si>
+    <t>TRIPOLI+F-12</t>
+  </si>
+  <si>
+    <t>SUBWAY+F-11</t>
+  </si>
+  <si>
+    <t>LA FONDA STA CLARA+F-10</t>
+  </si>
+  <si>
+    <t>LA CUEVA DEL ZORRO+F-9</t>
+  </si>
+  <si>
+    <t>SKUISITO+F-8</t>
+  </si>
+  <si>
+    <t>FOODSITE+F-7</t>
+  </si>
+  <si>
+    <t>FISH &amp; GAMBAS+F-4</t>
+  </si>
+  <si>
+    <t>LEBNAN+F-5</t>
+  </si>
+  <si>
+    <t>SCAPPINO+A-10</t>
+  </si>
+  <si>
+    <t>OUTLET DEPORTES 02+M-2</t>
+  </si>
+  <si>
+    <t>BIZARRO+C-7B</t>
+  </si>
+  <si>
+    <t>VICTORINOX+E-4</t>
+  </si>
+  <si>
+    <t>DOMINO'S+F-6B</t>
+  </si>
+  <si>
+    <t>SALEVALE+F-6A</t>
+  </si>
+  <si>
+    <t>LA CHINATA+G-1A</t>
+  </si>
+  <si>
+    <t>PERRY ELLIS+G-1B</t>
+  </si>
+  <si>
+    <t>ROCK HAMPTON+G-2</t>
+  </si>
+  <si>
+    <t>CUADRA+G-3</t>
+  </si>
+  <si>
+    <t>SPORT OUTLET+G-7, G-8</t>
+  </si>
+  <si>
+    <t>AREA CODE+N-7</t>
+  </si>
+  <si>
+    <t>VIPS+N-4</t>
+  </si>
+  <si>
+    <t>REEBOK+I-1</t>
+  </si>
+  <si>
+    <t>puerta</t>
+  </si>
+  <si>
+    <t>puerta (1)</t>
+  </si>
+  <si>
+    <t>puerta (2)</t>
+  </si>
+  <si>
+    <t>puerta (3)</t>
+  </si>
+  <si>
+    <t>puerta (4)</t>
+  </si>
+  <si>
+    <t>puerta (5)</t>
+  </si>
+  <si>
+    <t>puerta (6)</t>
+  </si>
+  <si>
+    <t>puerta (7)</t>
+  </si>
+  <si>
+    <t>banoHombres</t>
+  </si>
+  <si>
+    <t>banoMujeres</t>
+  </si>
+  <si>
+    <t>banoDoble</t>
+  </si>
+  <si>
+    <t>banoDoble (1)</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>isla-KRISPY KREME</t>
+  </si>
+  <si>
+    <t>isla (1)-DELSEY</t>
+  </si>
+  <si>
+    <t>isla (2)-ACCESORIOS MÓVILES</t>
+  </si>
+  <si>
+    <t>isla (3)-MITALLA</t>
+  </si>
+  <si>
+    <t>isla (4)-FRAGANCIAS EUROPEAS</t>
+  </si>
+  <si>
+    <t>isla (5)-VEINTI4</t>
+  </si>
+  <si>
+    <t>isla (6)-L'OCCITANE</t>
+  </si>
+  <si>
+    <t>isla (7)-SOXILION</t>
+  </si>
+  <si>
+    <t>isla (8)-AT&amp;T</t>
+  </si>
+  <si>
+    <t>isla (9)-SOLARIS</t>
+  </si>
+  <si>
+    <t>isla (10)-ACCESORIOS MÓVILES</t>
+  </si>
+  <si>
+    <t>isla (11)-SHYNE</t>
+  </si>
+  <si>
+    <t>isla (12)-GOC</t>
+  </si>
+  <si>
+    <t>isla (13)-BLACK PIRANHA</t>
+  </si>
+  <si>
+    <t>isla (14)-GABÍN</t>
+  </si>
+  <si>
+    <t>isla (15)-BASKIN ROBINS</t>
+  </si>
+  <si>
+    <t>isla (16)-BIANNE</t>
+  </si>
+  <si>
+    <t>isla (17) horizontal-ACCESORIOS MÓVILES</t>
+  </si>
+  <si>
+    <t>isla (18)-CANDY OUTLET</t>
+  </si>
+  <si>
+    <t>isla (19)-ACCESORIOS MÓVILES</t>
+  </si>
+  <si>
+    <t>isla (20)-SOLARIS</t>
+  </si>
+  <si>
+    <t>isla (21)-ACCESORIOS MÓVILES</t>
+  </si>
+  <si>
+    <t>isla (22) horizontal-SARI SILVER</t>
+  </si>
+  <si>
+    <t>isla (23) horizontal-SOLARIS</t>
+  </si>
+  <si>
+    <t>isla (24)-DOTIQUE</t>
+  </si>
+  <si>
+    <t>isla (25)-SHYNE</t>
+  </si>
+  <si>
+    <t>isla (26)  horizontal-SOLARIS</t>
+  </si>
+  <si>
+    <t>isla (27)-SWEET COLORS</t>
+  </si>
+  <si>
+    <t>isla (28) up-CANDY LAND</t>
+  </si>
+  <si>
+    <t>guiaColor</t>
+  </si>
+  <si>
+    <t>terminal</t>
+  </si>
+  <si>
+    <t>terminal (1)</t>
+  </si>
+  <si>
+    <t>terminal (2)</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1556,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1152,12 +1617,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1173,6 +1632,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1448,7 +1917,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1459,7 +1928,7 @@
   <dimension ref="A1:G409"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2166,26 +2635,24 @@
     <col min="16129" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2195,1225 +2662,867 @@
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="12" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="1:7" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="E5" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="11">
+        <v>2106659</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2106277</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="25">
+        <v>2105901</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2106017</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2106023</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2106669</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2319945</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2106132</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="E14" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="E15" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="25">
+        <v>2106280</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2106427</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2105350</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="9">
+        <v>2105319</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2105165</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="24">
+        <v>2319948</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="25">
+        <v>6889315</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="25">
+        <v>2106944</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="25">
+        <v>2106283</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2106338</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2105605</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="25">
+        <v>2105891</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="11">
+        <v>6889313</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="E32" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="11">
+        <v>2106030</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="11">
+        <v>2319958</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="25">
+        <v>2106295</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2106449</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="E39" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="11">
+        <v>2105939</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="25">
+        <v>2106468</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B44" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C44" s="24">
         <v>2105912</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E44" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C47" s="11">
+        <v>2106188</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" s="11">
+        <v>2106681</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2106075</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C50" s="11">
+        <v>2106198</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="25">
+        <v>2105491</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="25">
+        <v>2106155</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" s="20">
+        <v>2106048</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="11">
+        <v>2105836</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="11">
+        <v>2106103</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="27">
-        <v>2105901</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="27">
-        <v>2106000</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="14">
-        <v>2105693</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="27">
-        <v>2106506</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="27">
-        <v>2106400</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="27">
-        <v>2106283</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G9" s="15" t="s">
+      <c r="E57" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="11">
+        <v>2105935</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C60" s="11">
+        <v>2106664</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="27">
-        <v>2105491</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="B61" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="C61" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="27">
-        <v>2106280</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="27">
-        <v>2106155</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="27">
-        <v>2106023</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="G14" s="11">
-        <v>2105935</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="E61" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="11">
+        <v>2106122</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="11">
+        <v>2106446</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B65" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C65" s="25">
         <v>2106020</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="27">
-        <v>6889315</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="G16" s="11">
-        <v>2106278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="27">
-        <v>2106944</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G17" s="11">
-        <v>2106482</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="27">
-        <v>2106101</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G18" s="11">
-        <v>2105090</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="27">
-        <v>2106192</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="G19" s="11">
-        <v>2106075</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="11">
-        <v>2106030</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="G21" s="11">
-        <v>2105899</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="27">
-        <v>2105891</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="G22" s="11">
-        <v>6885801</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="27">
-        <v>2105278</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="26">
-        <v>2319948</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="G25" s="11">
-        <v>2319946</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="27">
-        <v>2106295</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="G26" s="11">
-        <v>2106427</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="27">
-        <v>2106456</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="G27" s="9">
-        <v>2106377</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="27">
-        <v>2106096</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="27">
-        <v>2106468</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G29" s="11">
-        <v>2106132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="27">
-        <v>2106025</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="G30" s="11">
-        <v>2106381</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" s="11">
-        <v>6889313</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="G32" s="11">
-        <v>2105165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="27">
-        <v>2106095</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G33" s="11">
-        <v>2319958</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="11">
-        <v>2106175</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="G34" s="11">
-        <v>2106659</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="11">
-        <v>2105836</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="9">
-        <v>6903012</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="11">
-        <v>2105280</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="11">
-        <v>2105939</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="G37" s="9">
-        <v>2106449</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="11">
-        <v>2106065</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="G38" s="9">
-        <v>2319963</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="11">
-        <v>2105594</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="12" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="11">
-        <v>2106122</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="G40" s="9">
-        <v>2106394</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="G41" s="11">
-        <v>2106681</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="G42" s="11">
-        <v>2106060</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="11">
-        <v>2106579</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="G43" s="11">
-        <v>2106198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="11">
-        <v>2106501</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="G44" s="11">
-        <v>2105634</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="11">
-        <v>2106174</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="G45" s="11">
-        <v>2106384</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="G46" s="11">
-        <v>2319945</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="11">
-        <v>2106565</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="G47" s="11">
-        <v>2106603</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="G48" s="11">
-        <v>2106188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="11">
-        <v>2106103</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="G49" s="11">
-        <v>2106338</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" s="11">
-        <v>2106017</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="G50" s="11">
-        <v>2106418</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="9">
-        <v>2105319</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="G51" s="11">
-        <v>2106399</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="11">
-        <v>2105999</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="G52" s="11">
-        <v>2106664</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="11">
-        <v>2106013</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="G53" s="11">
-        <v>2106048</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C54" s="20">
-        <v>2105350</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="G54" s="11"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G55" s="11">
-        <v>2105096</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="11">
-        <v>2106672</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="G56" s="11">
-        <v>2105605</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="G57" s="11">
-        <v>2106446</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="11"/>
-      <c r="E58" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G58" s="11">
-        <v>2105096</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="11">
-        <v>6885911</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="G59" s="11"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="G60" s="11"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C61" s="11">
-        <v>2106669</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" s="11">
-        <v>2105655</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C63" s="11">
-        <v>2106277</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G63" s="11">
-        <v>2105523</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="G64" s="11">
-        <v>2221628764</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="11">
-        <v>2105096</v>
+      <c r="E65" s="2" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -3426,491 +3535,1080 @@
       <c r="C66" s="9">
         <v>2106440</v>
       </c>
+      <c r="E66" s="2" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C67" s="9"/>
+      <c r="A67" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C67" s="11">
+        <v>2106603</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C68" s="9">
-        <v>2105327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>138</v>
+      <c r="A68" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="11">
+        <v>2106065</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C69" s="11">
-        <v>2105096</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="9"/>
-      <c r="B70" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C70" s="9"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C71" s="9"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C72" s="11"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>138</v>
+        <v>2106174</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="E71" s="22" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="25">
+        <v>2106506</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="C73" s="11">
-        <v>2105096</v>
+        <v>2105523</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>151</v>
+        <v>211</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="E74" s="22"/>
+        <v>212</v>
+      </c>
+      <c r="C74" s="9">
+        <v>2106377</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>414</v>
+      </c>
       <c r="F74" s="22"/>
       <c r="G74" s="23"/>
     </row>
     <row r="75" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E75" s="22"/>
+      <c r="A75" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" s="14">
+        <v>2105693</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>415</v>
+      </c>
       <c r="F75" s="22"/>
       <c r="G75" s="23"/>
     </row>
     <row r="76" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E76" s="22"/>
+      <c r="A76" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>406</v>
+      </c>
       <c r="F76" s="22"/>
       <c r="G76" s="23"/>
     </row>
     <row r="77" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A77" s="21"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="21"/>
+      <c r="A77" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" s="11">
+        <v>2106060</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>369</v>
+      </c>
       <c r="G77" s="23"/>
     </row>
     <row r="78" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="21"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="21"/>
+      <c r="A78" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="11">
+        <v>2106672</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="G78" s="23"/>
     </row>
     <row r="79" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="21"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="21"/>
+      <c r="A79" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="11">
+        <v>2105999</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>321</v>
+      </c>
       <c r="G79" s="23"/>
     </row>
     <row r="80" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="21"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="21"/>
+      <c r="A80" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80" s="25">
+        <v>2106095</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>333</v>
+      </c>
       <c r="G80" s="23"/>
     </row>
     <row r="81" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="21"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="21"/>
+      <c r="A81" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C81" s="11">
+        <v>2106418</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>303</v>
+      </c>
       <c r="G81" s="23"/>
     </row>
     <row r="82" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A82" s="21"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="21"/>
+      <c r="A82" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="G82" s="23"/>
     </row>
     <row r="83" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A83" s="21"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="21"/>
+      <c r="A83" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="C83" s="9">
+        <v>2319963</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>385</v>
+      </c>
       <c r="G83" s="23"/>
     </row>
     <row r="84" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="21"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="21"/>
+      <c r="A84" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>374</v>
+      </c>
       <c r="G84" s="23"/>
     </row>
     <row r="85" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A85" s="21"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="21"/>
+      <c r="A85" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C85" s="9">
+        <v>2105327</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>373</v>
+      </c>
       <c r="G85" s="23"/>
     </row>
     <row r="86" spans="1:7" s="22" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="21"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="21"/>
+      <c r="A86" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C86" s="11">
+        <v>2106384</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>345</v>
+      </c>
       <c r="G86" s="23"/>
     </row>
     <row r="87" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="21"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="21"/>
+      <c r="A87" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C87" s="11">
+        <v>2105634</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>378</v>
+      </c>
       <c r="G87" s="23"/>
     </row>
     <row r="88" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A88" s="21"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="21"/>
+      <c r="A88" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" s="11">
+        <v>2106175</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="G88" s="23"/>
     </row>
     <row r="89" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A89" s="21"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="21"/>
+      <c r="A89" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="11">
+        <v>2106579</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="G89" s="23"/>
     </row>
     <row r="90" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="21"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="21"/>
+      <c r="A90" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="G90" s="23"/>
     </row>
     <row r="91" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="21"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="21"/>
+      <c r="A91" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>337</v>
+      </c>
       <c r="G91" s="23"/>
     </row>
     <row r="92" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A92" s="21"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="21"/>
+      <c r="A92" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="E92" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="G92" s="23"/>
     </row>
     <row r="93" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A93" s="21"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="21"/>
+      <c r="A93" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="11">
+        <v>2106381</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G93" s="23"/>
     </row>
     <row r="94" spans="1:7" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="21"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="21"/>
+      <c r="A94" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>300</v>
+      </c>
       <c r="G94" s="23"/>
     </row>
     <row r="95" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A95" s="21"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="21"/>
+      <c r="A95" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" s="11">
+        <v>2105090</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="G95" s="23"/>
     </row>
     <row r="96" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="21"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="21"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="E96" s="2" t="s">
+        <v>346</v>
+      </c>
       <c r="G96" s="23"/>
     </row>
     <row r="97" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="21"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="21"/>
+      <c r="A97" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="E97" s="22" t="s">
+        <v>366</v>
+      </c>
       <c r="G97" s="23"/>
     </row>
     <row r="98" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="21"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="21"/>
+      <c r="A98" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="25">
+        <v>2106000</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>344</v>
+      </c>
       <c r="G98" s="23"/>
     </row>
     <row r="99" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="21"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="21"/>
+      <c r="A99" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>380</v>
+      </c>
       <c r="G99" s="23"/>
     </row>
     <row r="100" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="21"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="21"/>
+      <c r="A100" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100" s="11">
+        <v>2105096</v>
+      </c>
+      <c r="E100" s="22" t="s">
+        <v>358</v>
+      </c>
       <c r="G100" s="23"/>
     </row>
     <row r="101" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="21"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="21"/>
+      <c r="A101" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C101" s="11">
+        <v>2105096</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>354</v>
+      </c>
       <c r="G101" s="23"/>
     </row>
     <row r="102" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="21"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="21"/>
+      <c r="A102" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" s="11"/>
+      <c r="E102" s="22" t="s">
+        <v>386</v>
+      </c>
       <c r="G102" s="23"/>
     </row>
     <row r="103" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A103" s="21"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="21"/>
+      <c r="A103" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C103" s="11">
+        <v>2105096</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>334</v>
+      </c>
       <c r="G103" s="23"/>
     </row>
     <row r="104" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="21"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="21"/>
+      <c r="A104" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C104" s="11">
+        <v>2105096</v>
+      </c>
+      <c r="E104" s="22" t="s">
+        <v>393</v>
+      </c>
       <c r="G104" s="23"/>
     </row>
     <row r="105" spans="1:7" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="21"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="21"/>
+      <c r="A105" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C105" s="11">
+        <v>2105096</v>
+      </c>
+      <c r="E105" s="22" t="s">
+        <v>394</v>
+      </c>
       <c r="G105" s="23"/>
     </row>
     <row r="106" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="21"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="21"/>
+      <c r="A106" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C106" s="11">
+        <v>6885911</v>
+      </c>
+      <c r="E106" s="22" t="s">
+        <v>395</v>
+      </c>
       <c r="G106" s="23"/>
     </row>
     <row r="107" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A107" s="21"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="21"/>
+      <c r="A107" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C107" s="11">
+        <v>2105280</v>
+      </c>
+      <c r="E107" s="22" t="s">
+        <v>396</v>
+      </c>
       <c r="G107" s="23"/>
     </row>
     <row r="108" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A108" s="21"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="21"/>
+      <c r="A108" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C108" s="11">
+        <v>6885801</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>397</v>
+      </c>
       <c r="G108" s="23"/>
     </row>
     <row r="109" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A109" s="21"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="21"/>
+      <c r="A109" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E109" s="22" t="s">
+        <v>398</v>
+      </c>
       <c r="G109" s="23"/>
     </row>
     <row r="110" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="21"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="21"/>
+      <c r="A110" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>399</v>
+      </c>
       <c r="G110" s="23"/>
     </row>
     <row r="111" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A111" s="21"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="21"/>
+      <c r="A111" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C111" s="11">
+        <v>2106278</v>
+      </c>
+      <c r="E111" s="22" t="s">
+        <v>400</v>
+      </c>
       <c r="G111" s="23"/>
     </row>
     <row r="112" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A112" s="21"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="21"/>
+      <c r="A112" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C112" s="11">
+        <v>2106399</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="G112" s="23"/>
     </row>
     <row r="113" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="21"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="21"/>
+      <c r="A113" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="G113" s="23"/>
     </row>
     <row r="114" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A114" s="21"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="21"/>
+      <c r="A114" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C114" s="9">
+        <v>2106394</v>
+      </c>
+      <c r="E114" s="22" t="s">
+        <v>392</v>
+      </c>
       <c r="G114" s="23"/>
     </row>
     <row r="115" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="21"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="21"/>
+      <c r="A115" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B115" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C115" s="25">
+        <v>2105278</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="G115" s="23"/>
     </row>
     <row r="116" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A116" s="21"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="21"/>
+      <c r="A116" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B116" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C116" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>320</v>
+      </c>
       <c r="G116" s="23"/>
     </row>
     <row r="117" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A117" s="21"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="21"/>
+      <c r="A117" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="25">
+        <v>2106400</v>
+      </c>
+      <c r="E117" s="22" t="s">
+        <v>387</v>
+      </c>
       <c r="G117" s="23"/>
     </row>
     <row r="118" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A118" s="21"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="21"/>
+      <c r="A118" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C118" s="11">
+        <v>2105655</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="G118" s="23"/>
     </row>
     <row r="119" spans="1:7" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="21"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="21"/>
+      <c r="A119" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C119" s="11">
+        <v>2106482</v>
+      </c>
+      <c r="E119" s="22" t="s">
+        <v>384</v>
+      </c>
       <c r="G119" s="23"/>
     </row>
     <row r="120" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A120" s="21"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="21"/>
+      <c r="A120" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C120" s="11">
+        <v>2319946</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="G120" s="23"/>
     </row>
     <row r="121" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A121" s="21"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="21"/>
+      <c r="A121" s="11"/>
+      <c r="B121" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C121" s="11">
+        <v>2221628764</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="G121" s="23"/>
     </row>
     <row r="122" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A122" s="21"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="21"/>
+      <c r="A122" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C122" s="11">
+        <v>2106565</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G122" s="23"/>
     </row>
     <row r="123" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A123" s="21"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="21"/>
+      <c r="A123" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C123" s="11">
+        <v>2105899</v>
+      </c>
+      <c r="E123" s="22" t="s">
+        <v>379</v>
+      </c>
       <c r="G123" s="23"/>
     </row>
     <row r="124" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A124" s="21"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="21"/>
+      <c r="A124" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C124" s="11">
+        <v>2106013</v>
+      </c>
+      <c r="E124" s="22" t="s">
+        <v>370</v>
+      </c>
       <c r="G124" s="23"/>
     </row>
     <row r="125" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A125" s="21"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="21"/>
+      <c r="A125" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B125" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C125" s="25">
+        <v>2106101</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>308</v>
+      </c>
       <c r="G125" s="23"/>
     </row>
     <row r="126" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A126" s="21"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="21"/>
+      <c r="A126" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C126" s="11">
+        <v>2105594</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>309</v>
+      </c>
       <c r="G126" s="23"/>
     </row>
     <row r="127" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A127" s="21"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="21"/>
+      <c r="A127" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C127" s="11">
+        <v>2106501</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>299</v>
+      </c>
       <c r="G127" s="23"/>
     </row>
     <row r="128" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A128" s="21"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="21"/>
+      <c r="A128" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B128" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C128" s="25">
+        <v>2106025</v>
+      </c>
+      <c r="E128" s="22" t="s">
+        <v>375</v>
+      </c>
       <c r="G128" s="23"/>
     </row>
     <row r="129" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A129" s="21"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="21"/>
+      <c r="A129" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E129" s="22" t="s">
+        <v>389</v>
+      </c>
       <c r="G129" s="23"/>
     </row>
     <row r="130" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A130" s="21"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="21"/>
+      <c r="A130" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C130" s="25">
+        <v>2106192</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="G130" s="23"/>
     </row>
     <row r="131" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A131" s="21"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="21"/>
+      <c r="A131" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="G131" s="23"/>
     </row>
     <row r="132" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A132" s="21"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="21"/>
+      <c r="A132" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C132" s="25">
+        <v>2106456</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="G132" s="23"/>
     </row>
     <row r="133" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A133" s="21"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="21"/>
+      <c r="A133" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B133" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C133" s="25">
+        <v>2106096</v>
+      </c>
+      <c r="E133" s="22" t="s">
+        <v>372</v>
+      </c>
       <c r="G133" s="23"/>
     </row>
     <row r="134" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A134" s="21"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="21"/>
+      <c r="A134" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B134" s="10"/>
+      <c r="C134" s="11"/>
+      <c r="E134" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="G134" s="23"/>
     </row>
     <row r="135" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A135" s="21"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="21"/>
+      <c r="A135" s="17"/>
+      <c r="B135" s="17"/>
+      <c r="C135" s="9">
+        <v>6903012</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="G135" s="23"/>
     </row>
     <row r="136" spans="1:7" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="21"/>
       <c r="B136" s="2"/>
       <c r="C136" s="21"/>
+      <c r="E136" s="2" t="s">
+        <v>311</v>
+      </c>
       <c r="G136" s="23"/>
     </row>
     <row r="137" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137" s="21"/>
       <c r="B137" s="2"/>
       <c r="C137" s="21"/>
+      <c r="E137" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="G137" s="23"/>
     </row>
     <row r="138" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138" s="21"/>
       <c r="B138" s="2"/>
       <c r="C138" s="21"/>
+      <c r="E138" s="2" t="s">
+        <v>436</v>
+      </c>
       <c r="G138" s="23"/>
     </row>
     <row r="139" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139" s="21"/>
       <c r="B139" s="2"/>
       <c r="C139" s="21"/>
+      <c r="E139" s="2" t="s">
+        <v>437</v>
+      </c>
       <c r="G139" s="23"/>
     </row>
     <row r="140" spans="1:7" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="21"/>
       <c r="B140" s="2"/>
       <c r="C140" s="21"/>
+      <c r="E140" s="2" t="s">
+        <v>438</v>
+      </c>
       <c r="G140" s="23"/>
     </row>
     <row r="141" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141" s="21"/>
       <c r="B141" s="2"/>
       <c r="C141" s="21"/>
+      <c r="E141" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="G141" s="23"/>
     </row>
     <row r="142" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A142" s="21"/>
       <c r="B142" s="2"/>
       <c r="C142" s="21"/>
-      <c r="E142" s="2"/>
+      <c r="E142" s="22" t="s">
+        <v>367</v>
+      </c>
       <c r="F142" s="2"/>
       <c r="G142" s="21"/>
     </row>
@@ -3918,7 +4616,9 @@
       <c r="A143" s="6"/>
       <c r="B143" s="4"/>
       <c r="C143" s="6"/>
-      <c r="E143" s="2"/>
+      <c r="E143" s="22" t="s">
+        <v>371</v>
+      </c>
       <c r="F143" s="2"/>
       <c r="G143" s="21"/>
     </row>
@@ -3926,9 +4626,86 @@
       <c r="A144" s="6"/>
       <c r="B144" s="4"/>
       <c r="C144" s="6"/>
-      <c r="E144" s="2"/>
+      <c r="E144" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="F144" s="2"/>
       <c r="G144" s="21"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E145" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="146" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E146" s="22" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E147" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E148" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E149" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E150" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="151" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E151" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E152" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E153" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="154" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E154" s="22" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="155" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E155" s="22" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E156" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E157" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="158" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E158" s="22" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="159" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E159" s="22" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="409" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B409" s="2" t="s">
@@ -3936,12 +4713,12 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="I3:I158">
+    <sortCondition ref="I2"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G7:G25" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajusto los labels de los botones diagonales
</commit_message>
<xml_diff>
--- a/MapaOutlet/Assets/References/Directorio locales.xlsx
+++ b/MapaOutlet/Assets/References/Directorio locales.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -1629,9 +1630,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1642,6 +1640,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,7 +1918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1927,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2636,11 +2637,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -2662,23 +2663,20 @@
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:7" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>165</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2689,11 +2687,8 @@
         <v>152</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="E5" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>137</v>
       </c>
@@ -2702,9 +2697,6 @@
       </c>
       <c r="C6" s="11">
         <v>2106659</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2717,9 +2709,6 @@
       <c r="C7" s="11">
         <v>2106277</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>310</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
@@ -2731,11 +2720,8 @@
       <c r="C8" s="25">
         <v>2105901</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>106</v>
       </c>
@@ -2745,11 +2731,8 @@
       <c r="C9" s="11">
         <v>2106017</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>25</v>
       </c>
@@ -2759,11 +2742,8 @@
       <c r="C10" s="25">
         <v>2106023</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>129</v>
       </c>
@@ -2773,11 +2753,8 @@
       <c r="C11" s="11">
         <v>2106669</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>248</v>
       </c>
@@ -2787,11 +2764,8 @@
       <c r="C12" s="11">
         <v>2319945</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>135</v>
       </c>
@@ -2800,9 +2774,6 @@
       </c>
       <c r="C13" s="11">
         <v>2106132</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2813,9 +2784,6 @@
         <v>136</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="E14" s="2" t="s">
-        <v>335</v>
-      </c>
     </row>
     <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
@@ -2825,11 +2793,8 @@
         <v>276</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="E15" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>40</v>
       </c>
@@ -2839,11 +2804,8 @@
       <c r="C16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>18</v>
       </c>
@@ -2853,11 +2815,8 @@
       <c r="C17" s="25">
         <v>2106280</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>209</v>
       </c>
@@ -2867,11 +2826,8 @@
       <c r="C18" s="11">
         <v>2106427</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>114</v>
       </c>
@@ -2881,11 +2837,8 @@
       <c r="C19" s="11">
         <v>2105350</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>108</v>
       </c>
@@ -2895,11 +2848,8 @@
       <c r="C20" s="9">
         <v>2105319</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>221</v>
       </c>
@@ -2909,11 +2859,8 @@
       <c r="C21" s="11">
         <v>2105165</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>101</v>
       </c>
@@ -2923,11 +2870,8 @@
       <c r="C22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>50</v>
       </c>
@@ -2937,11 +2881,8 @@
       <c r="C23" s="24">
         <v>2319948</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>29</v>
       </c>
@@ -2951,11 +2892,8 @@
       <c r="C24" s="25">
         <v>6889315</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>31</v>
       </c>
@@ -2965,11 +2903,8 @@
       <c r="C25" s="25">
         <v>2106944</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>14</v>
       </c>
@@ -2979,11 +2914,8 @@
       <c r="C26" s="25">
         <v>2106283</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>254</v>
       </c>
@@ -2993,11 +2925,8 @@
       <c r="C27" s="11">
         <v>2106338</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>266</v>
       </c>
@@ -3007,11 +2936,8 @@
       <c r="C28" s="11">
         <v>2105605</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>43</v>
       </c>
@@ -3021,11 +2947,8 @@
       <c r="C29" s="25">
         <v>2105891</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>219</v>
       </c>
@@ -3035,11 +2958,8 @@
       <c r="C30" s="11">
         <v>6889313</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>173</v>
       </c>
@@ -3049,11 +2969,8 @@
       <c r="C31" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>147</v>
       </c>
@@ -3061,11 +2978,8 @@
         <v>148</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="E32" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>195</v>
       </c>
@@ -3075,11 +2989,8 @@
       <c r="C33" s="11">
         <v>2106030</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>223</v>
       </c>
@@ -3089,11 +3000,8 @@
       <c r="C34" s="11">
         <v>2319958</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>52</v>
       </c>
@@ -3103,11 +3011,8 @@
       <c r="C35" s="25">
         <v>2106295</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>167</v>
       </c>
@@ -3117,11 +3022,8 @@
       <c r="C36" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>229</v>
       </c>
@@ -3131,11 +3033,8 @@
       <c r="C37" s="9">
         <v>2106449</v>
       </c>
-      <c r="E37" s="22" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>176</v>
       </c>
@@ -3145,11 +3044,8 @@
       <c r="C38" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>271</v>
       </c>
@@ -3157,11 +3053,8 @@
         <v>272</v>
       </c>
       <c r="C39" s="11"/>
-      <c r="E39" s="22" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>161</v>
       </c>
@@ -3171,11 +3064,8 @@
       <c r="C40" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="22" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>76</v>
       </c>
@@ -3185,11 +3075,8 @@
       <c r="C41" s="11">
         <v>2105939</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
         <v>58</v>
       </c>
@@ -3199,11 +3086,8 @@
       <c r="C42" s="25">
         <v>2106468</v>
       </c>
-      <c r="E42" s="22" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>204</v>
       </c>
@@ -3213,11 +3097,8 @@
       <c r="C43" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="25" t="s">
         <v>4</v>
       </c>
@@ -3227,11 +3108,8 @@
       <c r="C44" s="24">
         <v>2105912</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>62</v>
       </c>
@@ -3241,11 +3119,8 @@
       <c r="C45" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>116</v>
       </c>
@@ -3255,11 +3130,8 @@
       <c r="C46" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>252</v>
       </c>
@@ -3269,11 +3141,8 @@
       <c r="C47" s="11">
         <v>2106188</v>
       </c>
-      <c r="E47" s="22" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>238</v>
       </c>
@@ -3283,11 +3152,8 @@
       <c r="C48" s="11">
         <v>2106681</v>
       </c>
-      <c r="E48" s="22" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>193</v>
       </c>
@@ -3297,11 +3163,8 @@
       <c r="C49" s="11">
         <v>2106075</v>
       </c>
-      <c r="E49" s="22" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>242</v>
       </c>
@@ -3311,11 +3174,8 @@
       <c r="C50" s="11">
         <v>2106198</v>
       </c>
-      <c r="E50" s="22" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
         <v>16</v>
       </c>
@@ -3325,11 +3185,8 @@
       <c r="C51" s="25">
         <v>2105491</v>
       </c>
-      <c r="E51" s="22" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
         <v>20</v>
       </c>
@@ -3339,11 +3196,8 @@
       <c r="C52" s="25">
         <v>2106155</v>
       </c>
-      <c r="E52" s="22" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>226</v>
       </c>
@@ -3353,11 +3207,8 @@
       <c r="C53" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E53" s="22" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>262</v>
       </c>
@@ -3367,11 +3218,8 @@
       <c r="C54" s="20">
         <v>2106048</v>
       </c>
-      <c r="E54" s="22" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>72</v>
       </c>
@@ -3381,11 +3229,8 @@
       <c r="C55" s="11">
         <v>2105836</v>
       </c>
-      <c r="E55" s="22" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>104</v>
       </c>
@@ -3395,11 +3240,8 @@
       <c r="C56" s="11">
         <v>2106103</v>
       </c>
-      <c r="E56" s="22" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>154</v>
       </c>
@@ -3409,11 +3251,8 @@
       <c r="C57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="22" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>182</v>
       </c>
@@ -3423,11 +3262,8 @@
       <c r="C58" s="11">
         <v>2105935</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>184</v>
       </c>
@@ -3437,11 +3273,8 @@
       <c r="C59" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E59" s="22" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>260</v>
       </c>
@@ -3451,11 +3284,8 @@
       <c r="C60" s="11">
         <v>2106664</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>170</v>
       </c>
@@ -3465,11 +3295,8 @@
       <c r="C61" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
         <v>47</v>
       </c>
@@ -3479,11 +3306,8 @@
       <c r="C62" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>82</v>
       </c>
@@ -3493,11 +3317,8 @@
       <c r="C63" s="11">
         <v>2106122</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>268</v>
       </c>
@@ -3506,9 +3327,6 @@
       </c>
       <c r="C64" s="11">
         <v>2106446</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3521,9 +3339,6 @@
       <c r="C65" s="25">
         <v>2106020</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>431</v>
-      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
@@ -3535,9 +3350,6 @@
       <c r="C66" s="9">
         <v>2106440</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>432</v>
-      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
@@ -3549,9 +3361,6 @@
       <c r="C67" s="11">
         <v>2106603</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>433</v>
-      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
@@ -3563,11 +3372,8 @@
       <c r="C68" s="11">
         <v>2106065</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>94</v>
       </c>
@@ -3577,11 +3383,8 @@
       <c r="C69" s="11">
         <v>2106174</v>
       </c>
-      <c r="E69" s="22" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>120</v>
       </c>
@@ -3591,11 +3394,8 @@
       <c r="C70" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E70" s="22" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>273</v>
       </c>
@@ -3603,11 +3403,8 @@
         <v>274</v>
       </c>
       <c r="C71" s="11"/>
-      <c r="E71" s="22" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="25" t="s">
         <v>10</v>
       </c>
@@ -3617,11 +3414,8 @@
       <c r="C72" s="25">
         <v>2106506</v>
       </c>
-      <c r="E72" s="22" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>280</v>
       </c>
@@ -3630,9 +3424,6 @@
       </c>
       <c r="C73" s="11">
         <v>2105523</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3645,9 +3436,6 @@
       <c r="C74" s="9">
         <v>2106377</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>414</v>
-      </c>
       <c r="F74" s="22"/>
       <c r="G74" s="23"/>
     </row>
@@ -3661,9 +3449,6 @@
       <c r="C75" s="14">
         <v>2105693</v>
       </c>
-      <c r="E75" s="22" t="s">
-        <v>415</v>
-      </c>
       <c r="F75" s="22"/>
       <c r="G75" s="23"/>
     </row>
@@ -3677,9 +3462,6 @@
       <c r="C76" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E76" s="22" t="s">
-        <v>406</v>
-      </c>
       <c r="F76" s="22"/>
       <c r="G76" s="23"/>
     </row>
@@ -3693,9 +3475,6 @@
       <c r="C77" s="11">
         <v>2106060</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>369</v>
-      </c>
       <c r="G77" s="23"/>
     </row>
     <row r="78" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3708,9 +3487,6 @@
       <c r="C78" s="11">
         <v>2106672</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="G78" s="23"/>
     </row>
     <row r="79" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3723,9 +3499,6 @@
       <c r="C79" s="11">
         <v>2105999</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="G79" s="23"/>
     </row>
     <row r="80" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3738,9 +3511,6 @@
       <c r="C80" s="25">
         <v>2106095</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="G80" s="23"/>
     </row>
     <row r="81" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3753,9 +3523,6 @@
       <c r="C81" s="11">
         <v>2106418</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="G81" s="23"/>
     </row>
     <row r="82" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3768,9 +3535,6 @@
       <c r="C82" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="G82" s="23"/>
     </row>
     <row r="83" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3783,9 +3547,6 @@
       <c r="C83" s="9">
         <v>2319963</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>385</v>
-      </c>
       <c r="G83" s="23"/>
     </row>
     <row r="84" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3798,9 +3559,6 @@
       <c r="C84" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>374</v>
-      </c>
       <c r="G84" s="23"/>
     </row>
     <row r="85" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3813,9 +3571,6 @@
       <c r="C85" s="9">
         <v>2105327</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>373</v>
-      </c>
       <c r="G85" s="23"/>
     </row>
     <row r="86" spans="1:7" s="22" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -3828,9 +3583,6 @@
       <c r="C86" s="11">
         <v>2106384</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="G86" s="23"/>
     </row>
     <row r="87" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3843,9 +3595,6 @@
       <c r="C87" s="11">
         <v>2105634</v>
       </c>
-      <c r="E87" s="22" t="s">
-        <v>378</v>
-      </c>
       <c r="G87" s="23"/>
     </row>
     <row r="88" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3858,9 +3607,6 @@
       <c r="C88" s="11">
         <v>2106175</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="G88" s="23"/>
     </row>
     <row r="89" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3873,9 +3619,6 @@
       <c r="C89" s="11">
         <v>2106579</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="G89" s="23"/>
     </row>
     <row r="90" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3888,9 +3631,6 @@
       <c r="C90" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="G90" s="23"/>
     </row>
     <row r="91" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3903,9 +3643,6 @@
       <c r="C91" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="G91" s="23"/>
     </row>
     <row r="92" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3916,9 +3653,6 @@
         <v>142</v>
       </c>
       <c r="C92" s="9"/>
-      <c r="E92" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="G92" s="23"/>
     </row>
     <row r="93" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3931,9 +3665,6 @@
       <c r="C93" s="11">
         <v>2106381</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="G93" s="23"/>
     </row>
     <row r="94" spans="1:7" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3946,9 +3677,6 @@
       <c r="C94" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="G94" s="23"/>
     </row>
     <row r="95" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3960,9 +3688,6 @@
       </c>
       <c r="C95" s="11">
         <v>2105090</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="G95" s="23"/>
     </row>
@@ -3972,9 +3697,6 @@
         <v>146</v>
       </c>
       <c r="C96" s="9"/>
-      <c r="E96" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="G96" s="23"/>
     </row>
     <row r="97" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -3985,9 +3707,6 @@
         <v>146</v>
       </c>
       <c r="C97" s="11"/>
-      <c r="E97" s="22" t="s">
-        <v>366</v>
-      </c>
       <c r="G97" s="23"/>
     </row>
     <row r="98" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4000,9 +3719,6 @@
       <c r="C98" s="25">
         <v>2106000</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>344</v>
-      </c>
       <c r="G98" s="23"/>
     </row>
     <row r="99" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4015,9 +3731,6 @@
       <c r="C99" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="E99" s="22" t="s">
-        <v>380</v>
-      </c>
       <c r="G99" s="23"/>
     </row>
     <row r="100" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4030,9 +3743,6 @@
       <c r="C100" s="11">
         <v>2105096</v>
       </c>
-      <c r="E100" s="22" t="s">
-        <v>358</v>
-      </c>
       <c r="G100" s="23"/>
     </row>
     <row r="101" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4045,9 +3755,6 @@
       <c r="C101" s="11">
         <v>2105096</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>354</v>
-      </c>
       <c r="G101" s="23"/>
     </row>
     <row r="102" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4058,9 +3765,6 @@
         <v>138</v>
       </c>
       <c r="C102" s="11"/>
-      <c r="E102" s="22" t="s">
-        <v>386</v>
-      </c>
       <c r="G102" s="23"/>
     </row>
     <row r="103" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4073,9 +3777,6 @@
       <c r="C103" s="11">
         <v>2105096</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="G103" s="23"/>
     </row>
     <row r="104" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4088,9 +3789,6 @@
       <c r="C104" s="11">
         <v>2105096</v>
       </c>
-      <c r="E104" s="22" t="s">
-        <v>393</v>
-      </c>
       <c r="G104" s="23"/>
     </row>
     <row r="105" spans="1:7" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -4103,9 +3801,6 @@
       <c r="C105" s="11">
         <v>2105096</v>
       </c>
-      <c r="E105" s="22" t="s">
-        <v>394</v>
-      </c>
       <c r="G105" s="23"/>
     </row>
     <row r="106" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4118,9 +3813,6 @@
       <c r="C106" s="11">
         <v>6885911</v>
       </c>
-      <c r="E106" s="22" t="s">
-        <v>395</v>
-      </c>
       <c r="G106" s="23"/>
     </row>
     <row r="107" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4133,9 +3825,6 @@
       <c r="C107" s="11">
         <v>2105280</v>
       </c>
-      <c r="E107" s="22" t="s">
-        <v>396</v>
-      </c>
       <c r="G107" s="23"/>
     </row>
     <row r="108" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4148,9 +3837,6 @@
       <c r="C108" s="11">
         <v>6885801</v>
       </c>
-      <c r="E108" s="22" t="s">
-        <v>397</v>
-      </c>
       <c r="G108" s="23"/>
     </row>
     <row r="109" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4163,9 +3849,6 @@
       <c r="C109" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="E109" s="22" t="s">
-        <v>398</v>
-      </c>
       <c r="G109" s="23"/>
     </row>
     <row r="110" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4178,9 +3861,6 @@
       <c r="C110" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E110" s="22" t="s">
-        <v>399</v>
-      </c>
       <c r="G110" s="23"/>
     </row>
     <row r="111" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4193,9 +3873,6 @@
       <c r="C111" s="11">
         <v>2106278</v>
       </c>
-      <c r="E111" s="22" t="s">
-        <v>400</v>
-      </c>
       <c r="G111" s="23"/>
     </row>
     <row r="112" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4208,9 +3885,6 @@
       <c r="C112" s="11">
         <v>2106399</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>356</v>
-      </c>
       <c r="G112" s="23"/>
     </row>
     <row r="113" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4223,9 +3897,6 @@
       <c r="C113" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="G113" s="23"/>
     </row>
     <row r="114" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4238,9 +3909,6 @@
       <c r="C114" s="9">
         <v>2106394</v>
       </c>
-      <c r="E114" s="22" t="s">
-        <v>392</v>
-      </c>
       <c r="G114" s="23"/>
     </row>
     <row r="115" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4253,9 +3921,6 @@
       <c r="C115" s="25">
         <v>2105278</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="G115" s="23"/>
     </row>
     <row r="116" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4268,9 +3933,6 @@
       <c r="C116" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="G116" s="23"/>
     </row>
     <row r="117" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4283,9 +3945,6 @@
       <c r="C117" s="25">
         <v>2106400</v>
       </c>
-      <c r="E117" s="22" t="s">
-        <v>387</v>
-      </c>
       <c r="G117" s="23"/>
     </row>
     <row r="118" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4298,9 +3957,6 @@
       <c r="C118" s="11">
         <v>2105655</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="G118" s="23"/>
     </row>
     <row r="119" spans="1:7" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4313,9 +3969,6 @@
       <c r="C119" s="11">
         <v>2106482</v>
       </c>
-      <c r="E119" s="22" t="s">
-        <v>384</v>
-      </c>
       <c r="G119" s="23"/>
     </row>
     <row r="120" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4327,9 +3980,6 @@
       </c>
       <c r="C120" s="11">
         <v>2319946</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="G120" s="23"/>
     </row>
@@ -4341,9 +3991,6 @@
       <c r="C121" s="11">
         <v>2221628764</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="G121" s="23"/>
     </row>
     <row r="122" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4356,9 +4003,6 @@
       <c r="C122" s="11">
         <v>2106565</v>
       </c>
-      <c r="E122" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="G122" s="23"/>
     </row>
     <row r="123" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4371,9 +4015,6 @@
       <c r="C123" s="11">
         <v>2105899</v>
       </c>
-      <c r="E123" s="22" t="s">
-        <v>379</v>
-      </c>
       <c r="G123" s="23"/>
     </row>
     <row r="124" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4386,9 +4027,6 @@
       <c r="C124" s="11">
         <v>2106013</v>
       </c>
-      <c r="E124" s="22" t="s">
-        <v>370</v>
-      </c>
       <c r="G124" s="23"/>
     </row>
     <row r="125" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4401,9 +4039,6 @@
       <c r="C125" s="25">
         <v>2106101</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="G125" s="23"/>
     </row>
     <row r="126" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4416,9 +4051,6 @@
       <c r="C126" s="11">
         <v>2105594</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="G126" s="23"/>
     </row>
     <row r="127" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4431,9 +4063,6 @@
       <c r="C127" s="11">
         <v>2106501</v>
       </c>
-      <c r="E127" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="G127" s="23"/>
     </row>
     <row r="128" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4446,9 +4075,6 @@
       <c r="C128" s="25">
         <v>2106025</v>
       </c>
-      <c r="E128" s="22" t="s">
-        <v>375</v>
-      </c>
       <c r="G128" s="23"/>
     </row>
     <row r="129" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4461,9 +4087,6 @@
       <c r="C129" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E129" s="22" t="s">
-        <v>389</v>
-      </c>
       <c r="G129" s="23"/>
     </row>
     <row r="130" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4476,9 +4099,6 @@
       <c r="C130" s="25">
         <v>2106192</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="G130" s="23"/>
     </row>
     <row r="131" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4491,9 +4111,6 @@
       <c r="C131" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="E131" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="G131" s="23"/>
     </row>
     <row r="132" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4506,9 +4123,6 @@
       <c r="C132" s="25">
         <v>2106456</v>
       </c>
-      <c r="E132" s="2" t="s">
-        <v>352</v>
-      </c>
       <c r="G132" s="23"/>
     </row>
     <row r="133" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4521,9 +4135,6 @@
       <c r="C133" s="25">
         <v>2106096</v>
       </c>
-      <c r="E133" s="22" t="s">
-        <v>372</v>
-      </c>
       <c r="G133" s="23"/>
     </row>
     <row r="134" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4532,9 +4143,6 @@
       </c>
       <c r="B134" s="10"/>
       <c r="C134" s="11"/>
-      <c r="E134" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="G134" s="23"/>
     </row>
     <row r="135" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -4543,72 +4151,48 @@
       <c r="C135" s="9">
         <v>6903012</v>
       </c>
-      <c r="E135" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="G135" s="23"/>
     </row>
     <row r="136" spans="1:7" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="21"/>
       <c r="B136" s="2"/>
       <c r="C136" s="21"/>
-      <c r="E136" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="G136" s="23"/>
     </row>
     <row r="137" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137" s="21"/>
       <c r="B137" s="2"/>
       <c r="C137" s="21"/>
-      <c r="E137" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="G137" s="23"/>
     </row>
     <row r="138" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138" s="21"/>
       <c r="B138" s="2"/>
       <c r="C138" s="21"/>
-      <c r="E138" s="2" t="s">
-        <v>436</v>
-      </c>
       <c r="G138" s="23"/>
     </row>
     <row r="139" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139" s="21"/>
       <c r="B139" s="2"/>
       <c r="C139" s="21"/>
-      <c r="E139" s="2" t="s">
-        <v>437</v>
-      </c>
       <c r="G139" s="23"/>
     </row>
     <row r="140" spans="1:7" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="21"/>
       <c r="B140" s="2"/>
       <c r="C140" s="21"/>
-      <c r="E140" s="2" t="s">
-        <v>438</v>
-      </c>
       <c r="G140" s="23"/>
     </row>
     <row r="141" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141" s="21"/>
       <c r="B141" s="2"/>
       <c r="C141" s="21"/>
-      <c r="E141" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="G141" s="23"/>
     </row>
     <row r="142" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A142" s="21"/>
       <c r="B142" s="2"/>
       <c r="C142" s="21"/>
-      <c r="E142" s="22" t="s">
-        <v>367</v>
-      </c>
       <c r="F142" s="2"/>
       <c r="G142" s="21"/>
     </row>
@@ -4616,9 +4200,6 @@
       <c r="A143" s="6"/>
       <c r="B143" s="4"/>
       <c r="C143" s="6"/>
-      <c r="E143" s="22" t="s">
-        <v>371</v>
-      </c>
       <c r="F143" s="2"/>
       <c r="G143" s="21"/>
     </row>
@@ -4626,86 +4207,8 @@
       <c r="A144" s="6"/>
       <c r="B144" s="4"/>
       <c r="C144" s="6"/>
-      <c r="E144" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="F144" s="2"/>
       <c r="G144" s="21"/>
-    </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E145" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="146" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E146" s="22" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E147" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E148" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E149" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E150" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="151" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E151" s="22" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E152" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E153" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="154" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E154" s="22" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="155" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E155" s="22" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E156" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E157" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="158" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E158" s="22" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="159" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E159" s="22" t="s">
-        <v>364</v>
-      </c>
     </row>
     <row r="409" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B409" s="2" t="s">
@@ -4720,5 +4223,801 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A156"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A156"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="22" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="22" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="22" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="22" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="22" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="22" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="22" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="22" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="22" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="22" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="22" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="22" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="22" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="22" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="22" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="22" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="22" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="22" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="22" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="22" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="22" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="22" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="22" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="22" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="22" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="22" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="22" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="22" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="22" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="22" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="22" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="22" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="22" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="22" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="22" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Agrego algunos datos de las tiendas al XML
</commit_message>
<xml_diff>
--- a/MapaOutlet/Assets/References/Directorio locales.xlsx
+++ b/MapaOutlet/Assets/References/Directorio locales.xlsx
@@ -298,9 +298,6 @@
     <t>ROCK PORT</t>
   </si>
   <si>
-    <t xml:space="preserve">I-3  </t>
-  </si>
-  <si>
     <t>VICKY FORM</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
   </si>
   <si>
     <t>F-11</t>
-  </si>
-  <si>
-    <t>SUB WAY</t>
   </si>
   <si>
     <t>F-12</t>
@@ -1387,12 +1381,18 @@
   <si>
     <t>terminal (2)</t>
   </si>
+  <si>
+    <t>SUBWAY</t>
+  </si>
+  <si>
+    <t>I-3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1434,8 +1434,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1445,6 +1452,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1557,7 +1570,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1574,12 +1587,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1643,6 +1650,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1918,7 +1940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1928,18 +1950,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="19" customWidth="1"/>
     <col min="4" max="5" width="11.44140625" style="2"/>
     <col min="6" max="6" width="20.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="19" customWidth="1"/>
     <col min="8" max="246" width="11.44140625" style="2"/>
     <col min="247" max="247" width="6.6640625" style="2" customWidth="1"/>
     <col min="248" max="248" width="18.6640625" style="2" customWidth="1"/>
@@ -2637,11 +2659,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -2649,1575 +2672,1677 @@
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="A3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="34">
+        <v>2105912</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="23">
+        <v>2105901</v>
+      </c>
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2106000</v>
+      </c>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2106506</v>
+      </c>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="23">
+        <v>2106400</v>
+      </c>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="23">
+        <v>2106283</v>
+      </c>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2105491</v>
+      </c>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="23">
+        <v>2106280</v>
+      </c>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2106155</v>
+      </c>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="23">
+        <v>2106023</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="23">
+        <v>2106020</v>
+      </c>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="23">
+        <v>6889315</v>
+      </c>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="23">
+        <v>2106944</v>
+      </c>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="23">
+        <v>2106101</v>
+      </c>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="23">
+        <v>2106192</v>
+      </c>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="23">
+        <v>2105891</v>
+      </c>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="23">
+        <v>2105278</v>
+      </c>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="25" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="22">
+        <v>2319948</v>
+      </c>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="23">
+        <v>2106295</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="23">
+        <v>2106456</v>
+      </c>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="23">
+        <v>2106096</v>
+      </c>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="23">
+        <v>2106468</v>
+      </c>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="23">
+        <v>2106025</v>
+      </c>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="12">
+        <v>2105693</v>
+      </c>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="35"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="C36" s="9">
+        <v>2106278</v>
+      </c>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2106482</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2105090</v>
+      </c>
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2106075</v>
+      </c>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2106030</v>
+      </c>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="35"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C42" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" s="11">
-        <v>2106659</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="11">
-        <v>2106277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="25">
-        <v>2105901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="11">
-        <v>2106017</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2106023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="11">
-        <v>2106669</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="C12" s="11">
-        <v>2319945</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C13" s="11">
-        <v>2106132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="25">
-        <v>2106280</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C18" s="11">
-        <v>2106427</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="11">
-        <v>2105350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="9">
-        <v>2105319</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C21" s="11">
-        <v>2105165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="B43" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" s="35"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D46" s="35"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" s="9">
+        <v>2105935</v>
+      </c>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="23">
+        <v>2106095</v>
+      </c>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="9">
+        <v>2106175</v>
+      </c>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="9">
+        <v>2105836</v>
+      </c>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="9">
+        <v>2105280</v>
+      </c>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="9">
+        <v>2105939</v>
+      </c>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="18">
+        <v>2106065</v>
+      </c>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="9">
+        <v>2105594</v>
+      </c>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" s="9">
+        <v>2106122</v>
+      </c>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="35"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="9">
+        <v>2106579</v>
+      </c>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="9">
+        <v>2106501</v>
+      </c>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="9">
+        <v>2106174</v>
+      </c>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="9">
+        <v>2106565</v>
+      </c>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="24">
-        <v>2319948</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="25">
-        <v>6889315</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="25">
-        <v>2106944</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="25">
-        <v>2106283</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C27" s="11">
-        <v>2106338</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="11">
-        <v>2105605</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="25">
-        <v>2105891</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="C30" s="11">
-        <v>6889313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C33" s="11">
-        <v>2106030</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C34" s="11">
-        <v>2319958</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="25">
-        <v>2106295</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="C37" s="9">
-        <v>2106449</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="11">
-        <v>2105939</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="25">
-        <v>2106468</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="24">
-        <v>2105912</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C47" s="11">
-        <v>2106188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="C48" s="11">
-        <v>2106681</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C49" s="11">
-        <v>2106075</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C50" s="11">
-        <v>2106198</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="25">
-        <v>2105491</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="25">
-        <v>2106155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C54" s="20">
-        <v>2106048</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="11">
-        <v>2105836</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
+      <c r="B65" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="11">
+      <c r="C65" s="9">
         <v>2106103</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" s="11">
-        <v>2105935</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C60" s="11">
-        <v>2106664</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="11">
-        <v>2106122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C64" s="11">
-        <v>2106446</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C65" s="25">
-        <v>2106020</v>
-      </c>
+      <c r="D65" s="35"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>140</v>
+        <v>105</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="C66" s="9">
-        <v>2106440</v>
-      </c>
+        <v>2106017</v>
+      </c>
+      <c r="D66" s="35"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C67" s="11">
-        <v>2106603</v>
-      </c>
+      <c r="A67" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2105319</v>
+      </c>
+      <c r="D67" s="35"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C68" s="11">
-        <v>2106065</v>
-      </c>
+      <c r="A68" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2105999</v>
+      </c>
+      <c r="D68" s="35"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="11">
-        <v>2106174</v>
-      </c>
+      <c r="A69" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2106013</v>
+      </c>
+      <c r="D69" s="35"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>122</v>
-      </c>
+      <c r="A70" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="9">
+        <v>2105350</v>
+      </c>
+      <c r="D70" s="35"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C71" s="11"/>
+      <c r="A71" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="35"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="25">
-        <v>2106506</v>
-      </c>
+      <c r="A72" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="35"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="11">
-        <v>2105523</v>
-      </c>
+      <c r="A73" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="9">
+        <v>2106672</v>
+      </c>
+      <c r="D73" s="35"/>
     </row>
     <row r="74" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" s="35"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="21"/>
+    </row>
+    <row r="75" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="35"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="21"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="9">
+        <v>6885911</v>
+      </c>
+      <c r="D76" s="35"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="36"/>
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="9">
+        <v>2106669</v>
+      </c>
+      <c r="D78" s="36"/>
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C79" s="9">
+        <v>2105655</v>
+      </c>
+      <c r="D79" s="36"/>
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80" s="9">
+        <v>2106277</v>
+      </c>
+      <c r="D80" s="36"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" s="9">
+        <v>2105899</v>
+      </c>
+      <c r="D81" s="36"/>
+      <c r="G81" s="21"/>
+    </row>
+    <row r="82" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" s="9">
+        <v>6885801</v>
+      </c>
+      <c r="D82" s="36"/>
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D83" s="36"/>
+      <c r="G83" s="21"/>
+    </row>
+    <row r="84" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A84" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D84" s="36"/>
+      <c r="G84" s="21"/>
+    </row>
+    <row r="85" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C85" s="9">
+        <v>2319946</v>
+      </c>
+      <c r="D85" s="36"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="1:7" s="20" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" s="9">
+        <v>2106427</v>
+      </c>
+      <c r="D86" s="36"/>
+      <c r="G86" s="21"/>
+    </row>
+    <row r="87" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2106377</v>
+      </c>
+      <c r="D87" s="36"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A88" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B88" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C74" s="9">
-        <v>2106377</v>
-      </c>
-      <c r="F74" s="22"/>
-      <c r="G74" s="23"/>
-    </row>
-    <row r="75" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C75" s="14">
-        <v>2105693</v>
-      </c>
-      <c r="F75" s="22"/>
-      <c r="G75" s="23"/>
-    </row>
-    <row r="76" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A76" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B76" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F76" s="22"/>
-      <c r="G76" s="23"/>
-    </row>
-    <row r="77" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A77" s="11" t="s">
+      <c r="C88" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D88" s="36"/>
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A89" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C89" s="9">
+        <v>2106132</v>
+      </c>
+      <c r="D89" s="36"/>
+      <c r="G89" s="21"/>
+    </row>
+    <row r="90" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A90" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="36"/>
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" s="9">
+        <v>2106381</v>
+      </c>
+      <c r="D91" s="36"/>
+      <c r="G91" s="21"/>
+    </row>
+    <row r="92" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="9">
+        <v>6889313</v>
+      </c>
+      <c r="D92" s="36"/>
+      <c r="G92" s="21"/>
+    </row>
+    <row r="93" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A93" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C93" s="9">
+        <v>2105165</v>
+      </c>
+      <c r="D93" s="36"/>
+      <c r="G93" s="21"/>
+    </row>
+    <row r="94" spans="1:7" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" s="9">
+        <v>2319958</v>
+      </c>
+      <c r="D94" s="36"/>
+      <c r="G94" s="21"/>
+    </row>
+    <row r="95" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C95" s="9">
+        <v>2106659</v>
+      </c>
+      <c r="D95" s="36"/>
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A96" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" s="9">
+        <v>2105096</v>
+      </c>
+      <c r="D96" s="36"/>
+      <c r="G96" s="21"/>
+    </row>
+    <row r="97" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A97" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D97" s="36"/>
+      <c r="G97" s="21"/>
+    </row>
+    <row r="98" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C98" s="7">
+        <v>2106449</v>
+      </c>
+      <c r="D98" s="36"/>
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C99" s="9">
+        <v>2106603</v>
+      </c>
+      <c r="D99" s="36"/>
+      <c r="G99" s="21"/>
+    </row>
+    <row r="100" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A100" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="7">
+        <v>2319963</v>
+      </c>
+      <c r="D100" s="36"/>
+      <c r="G100" s="21"/>
+    </row>
+    <row r="101" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A101" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D101" s="36"/>
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A102" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C102" s="7">
+        <v>2106394</v>
+      </c>
+      <c r="D102" s="37"/>
+      <c r="G102" s="21"/>
+    </row>
+    <row r="103" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C103" s="9">
+        <v>2106681</v>
+      </c>
+      <c r="D103" s="36"/>
+      <c r="G103" s="21"/>
+    </row>
+    <row r="104" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A104" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C104" s="9">
+        <v>2106060</v>
+      </c>
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" spans="1:7" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B105" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C77" s="11">
-        <v>2106060</v>
-      </c>
-      <c r="G77" s="23"/>
-    </row>
-    <row r="78" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="11">
-        <v>2106672</v>
-      </c>
-      <c r="G78" s="23"/>
-    </row>
-    <row r="79" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="11">
-        <v>2105999</v>
-      </c>
-      <c r="G79" s="23"/>
-    </row>
-    <row r="80" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C80" s="25">
-        <v>2106095</v>
-      </c>
-      <c r="G80" s="23"/>
-    </row>
-    <row r="81" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
+      <c r="C105" s="9">
+        <v>2106198</v>
+      </c>
+      <c r="G105" s="21"/>
+    </row>
+    <row r="106" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A106" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C106" s="9">
+        <v>2105634</v>
+      </c>
+      <c r="G106" s="21"/>
+    </row>
+    <row r="107" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A107" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C107" s="9">
+        <v>2106384</v>
+      </c>
+      <c r="G107" s="21"/>
+    </row>
+    <row r="108" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="9">
+        <v>2319945</v>
+      </c>
+      <c r="G108" s="21"/>
+    </row>
+    <row r="109" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" s="9">
+        <v>2106188</v>
+      </c>
+      <c r="G109" s="21"/>
+    </row>
+    <row r="110" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A110" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="9">
+        <v>2106338</v>
+      </c>
+      <c r="G110" s="21"/>
+    </row>
+    <row r="111" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C111" s="9">
+        <v>2106418</v>
+      </c>
+      <c r="G111" s="21"/>
+    </row>
+    <row r="112" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A112" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B112" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C81" s="11">
-        <v>2106418</v>
-      </c>
-      <c r="G81" s="23"/>
-    </row>
-    <row r="82" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A82" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B82" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G82" s="23"/>
-    </row>
-    <row r="83" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A83" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C83" s="9">
-        <v>2319963</v>
-      </c>
-      <c r="G83" s="23"/>
-    </row>
-    <row r="84" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G84" s="23"/>
-    </row>
-    <row r="85" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A85" s="9" t="s">
+      <c r="C112" s="9">
+        <v>2106399</v>
+      </c>
+      <c r="G112" s="21"/>
+    </row>
+    <row r="113" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A113" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C113" s="9">
+        <v>2106664</v>
+      </c>
+      <c r="G113" s="21"/>
+    </row>
+    <row r="114" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C114" s="7">
+        <v>2106440</v>
+      </c>
+      <c r="G114" s="21"/>
+    </row>
+    <row r="115" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A115" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="G115" s="21"/>
+    </row>
+    <row r="116" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A116" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C116" s="9"/>
+      <c r="G116" s="21"/>
+    </row>
+    <row r="117" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A117" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C117" s="9"/>
+      <c r="G117" s="21"/>
+    </row>
+    <row r="118" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A118" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C118" s="9">
+        <v>2106048</v>
+      </c>
+      <c r="G118" s="21"/>
+    </row>
+    <row r="119" spans="1:7" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="G119" s="21"/>
+    </row>
+    <row r="120" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A120" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C120" s="9">
+        <v>2105096</v>
+      </c>
+      <c r="G120" s="21"/>
+    </row>
+    <row r="121" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A121" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C121" s="9">
+        <v>2105605</v>
+      </c>
+      <c r="G121" s="21"/>
+    </row>
+    <row r="122" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C122" s="9">
+        <v>2106446</v>
+      </c>
+      <c r="G122" s="21"/>
+    </row>
+    <row r="123" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A123" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" s="9">
+        <v>2105096</v>
+      </c>
+      <c r="G123" s="21"/>
+    </row>
+    <row r="124" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A124" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G124" s="21"/>
+    </row>
+    <row r="125" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A125" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="9">
+        <v>2105523</v>
+      </c>
+      <c r="G125" s="21"/>
+    </row>
+    <row r="126" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C126" s="7"/>
+      <c r="G126" s="21"/>
+    </row>
+    <row r="127" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C127" s="7"/>
+      <c r="G127" s="21"/>
+    </row>
+    <row r="128" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="C128" s="7">
+        <v>2105327</v>
+      </c>
+      <c r="G128" s="21"/>
+    </row>
+    <row r="129" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C85" s="9">
-        <v>2105327</v>
-      </c>
-      <c r="G85" s="23"/>
-    </row>
-    <row r="86" spans="1:7" s="22" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C86" s="11">
-        <v>2106384</v>
-      </c>
-      <c r="G86" s="23"/>
-    </row>
-    <row r="87" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="C87" s="11">
-        <v>2105634</v>
-      </c>
-      <c r="G87" s="23"/>
-    </row>
-    <row r="88" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A88" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C88" s="11">
-        <v>2106175</v>
-      </c>
-      <c r="G88" s="23"/>
-    </row>
-    <row r="89" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A89" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C89" s="11">
-        <v>2106579</v>
-      </c>
-      <c r="G89" s="23"/>
-    </row>
-    <row r="90" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="B90" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G90" s="23"/>
-    </row>
-    <row r="91" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G91" s="23"/>
-    </row>
-    <row r="92" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A92" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B92" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C92" s="9"/>
-      <c r="G92" s="23"/>
-    </row>
-    <row r="93" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A93" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" s="11">
-        <v>2106381</v>
-      </c>
-      <c r="G93" s="23"/>
-    </row>
-    <row r="94" spans="1:7" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="G94" s="23"/>
-    </row>
-    <row r="95" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A95" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B95" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="11">
-        <v>2105090</v>
-      </c>
-      <c r="G95" s="23"/>
-    </row>
-    <row r="96" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="9"/>
-      <c r="B96" s="16" t="s">
+      <c r="B129" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C129" s="9">
+        <v>2105096</v>
+      </c>
+      <c r="G129" s="21"/>
+    </row>
+    <row r="130" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C96" s="9"/>
-      <c r="G96" s="23"/>
-    </row>
-    <row r="97" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="B97" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C97" s="11"/>
-      <c r="G97" s="23"/>
-    </row>
-    <row r="98" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B98" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" s="25">
-        <v>2106000</v>
-      </c>
-      <c r="G98" s="23"/>
-    </row>
-    <row r="99" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="G99" s="23"/>
-    </row>
-    <row r="100" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="11" t="s">
+      <c r="B130" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C130" s="7"/>
+      <c r="G130" s="21"/>
+    </row>
+    <row r="131" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A131" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B131" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C100" s="11">
+      <c r="C131" s="9"/>
+      <c r="G131" s="21"/>
+    </row>
+    <row r="132" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A132" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C132" s="9">
         <v>2105096</v>
       </c>
-      <c r="G100" s="23"/>
-    </row>
-    <row r="101" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="9" t="s">
+      <c r="G132" s="21"/>
+    </row>
+    <row r="133" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+      <c r="B133" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B101" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C101" s="11">
-        <v>2105096</v>
-      </c>
-      <c r="G101" s="23"/>
-    </row>
-    <row r="102" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B102" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C102" s="11"/>
-      <c r="G102" s="23"/>
-    </row>
-    <row r="103" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A103" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B103" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C103" s="11">
-        <v>2105096</v>
-      </c>
-      <c r="G103" s="23"/>
-    </row>
-    <row r="104" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="B104" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C104" s="11">
-        <v>2105096</v>
-      </c>
-      <c r="G104" s="23"/>
-    </row>
-    <row r="105" spans="1:7" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="B105" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C105" s="11">
-        <v>2105096</v>
-      </c>
-      <c r="G105" s="23"/>
-    </row>
-    <row r="106" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B106" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C106" s="11">
-        <v>6885911</v>
-      </c>
-      <c r="G106" s="23"/>
-    </row>
-    <row r="107" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A107" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C107" s="11">
-        <v>2105280</v>
-      </c>
-      <c r="G107" s="23"/>
-    </row>
-    <row r="108" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A108" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C108" s="11">
-        <v>6885801</v>
-      </c>
-      <c r="G108" s="23"/>
-    </row>
-    <row r="109" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A109" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C109" s="11" t="s">
+      <c r="C133" s="7"/>
+      <c r="G133" s="21"/>
+    </row>
+    <row r="134" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A134" s="9"/>
+      <c r="B134" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="G109" s="23"/>
-    </row>
-    <row r="110" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G110" s="23"/>
-    </row>
-    <row r="111" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A111" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C111" s="11">
-        <v>2106278</v>
-      </c>
-      <c r="G111" s="23"/>
-    </row>
-    <row r="112" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A112" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C112" s="11">
-        <v>2106399</v>
-      </c>
-      <c r="G112" s="23"/>
-    </row>
-    <row r="113" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="G113" s="23"/>
-    </row>
-    <row r="114" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A114" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B114" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="C114" s="9">
-        <v>2106394</v>
-      </c>
-      <c r="G114" s="23"/>
-    </row>
-    <row r="115" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B115" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C115" s="25">
-        <v>2105278</v>
-      </c>
-      <c r="G115" s="23"/>
-    </row>
-    <row r="116" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A116" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B116" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C116" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G116" s="23"/>
-    </row>
-    <row r="117" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A117" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B117" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C117" s="25">
-        <v>2106400</v>
-      </c>
-      <c r="G117" s="23"/>
-    </row>
-    <row r="118" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A118" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B118" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C118" s="11">
-        <v>2105655</v>
-      </c>
-      <c r="G118" s="23"/>
-    </row>
-    <row r="119" spans="1:7" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C119" s="11">
-        <v>2106482</v>
-      </c>
-      <c r="G119" s="23"/>
-    </row>
-    <row r="120" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A120" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B120" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C120" s="11">
-        <v>2319946</v>
-      </c>
-      <c r="G120" s="23"/>
-    </row>
-    <row r="121" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A121" s="11"/>
-      <c r="B121" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C121" s="11">
+      <c r="C134" s="9">
         <v>2221628764</v>
       </c>
-      <c r="G121" s="23"/>
-    </row>
-    <row r="122" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A122" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B122" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C122" s="11">
-        <v>2106565</v>
-      </c>
-      <c r="G122" s="23"/>
-    </row>
-    <row r="123" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A123" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B123" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C123" s="11">
-        <v>2105899</v>
-      </c>
-      <c r="G123" s="23"/>
-    </row>
-    <row r="124" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A124" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B124" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C124" s="11">
-        <v>2106013</v>
-      </c>
-      <c r="G124" s="23"/>
-    </row>
-    <row r="125" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A125" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B125" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C125" s="25">
-        <v>2106101</v>
-      </c>
-      <c r="G125" s="23"/>
-    </row>
-    <row r="126" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A126" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B126" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C126" s="11">
-        <v>2105594</v>
-      </c>
-      <c r="G126" s="23"/>
-    </row>
-    <row r="127" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A127" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B127" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C127" s="11">
-        <v>2106501</v>
-      </c>
-      <c r="G127" s="23"/>
-    </row>
-    <row r="128" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A128" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B128" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C128" s="25">
-        <v>2106025</v>
-      </c>
-      <c r="G128" s="23"/>
-    </row>
-    <row r="129" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A129" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B129" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G129" s="23"/>
-    </row>
-    <row r="130" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A130" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B130" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C130" s="25">
-        <v>2106192</v>
-      </c>
-      <c r="G130" s="23"/>
-    </row>
-    <row r="131" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A131" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B131" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C131" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="G131" s="23"/>
-    </row>
-    <row r="132" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A132" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B132" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C132" s="25">
-        <v>2106456</v>
-      </c>
-      <c r="G132" s="23"/>
-    </row>
-    <row r="133" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A133" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B133" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C133" s="25">
-        <v>2106096</v>
-      </c>
-      <c r="G133" s="23"/>
-    </row>
-    <row r="134" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A134" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B134" s="10"/>
-      <c r="C134" s="11"/>
-      <c r="G134" s="23"/>
-    </row>
-    <row r="135" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A135" s="17"/>
-      <c r="B135" s="17"/>
-      <c r="C135" s="9">
+      <c r="G134" s="21"/>
+    </row>
+    <row r="135" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A135" s="15"/>
+      <c r="B135" s="15"/>
+      <c r="C135" s="7">
         <v>6903012</v>
       </c>
-      <c r="G135" s="23"/>
-    </row>
-    <row r="136" spans="1:7" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="21"/>
+      <c r="G135" s="21"/>
+    </row>
+    <row r="136" spans="1:7" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="19"/>
       <c r="B136" s="2"/>
-      <c r="C136" s="21"/>
-      <c r="G136" s="23"/>
-    </row>
-    <row r="137" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A137" s="21"/>
+      <c r="C136" s="19"/>
+      <c r="G136" s="21"/>
+    </row>
+    <row r="137" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A137" s="19"/>
       <c r="B137" s="2"/>
-      <c r="C137" s="21"/>
-      <c r="G137" s="23"/>
-    </row>
-    <row r="138" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A138" s="21"/>
+      <c r="C137" s="19"/>
+      <c r="G137" s="21"/>
+    </row>
+    <row r="138" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A138" s="19"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="21"/>
-      <c r="G138" s="23"/>
-    </row>
-    <row r="139" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A139" s="21"/>
+      <c r="C138" s="19"/>
+      <c r="G138" s="21"/>
+    </row>
+    <row r="139" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A139" s="19"/>
       <c r="B139" s="2"/>
-      <c r="C139" s="21"/>
-      <c r="G139" s="23"/>
-    </row>
-    <row r="140" spans="1:7" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="21"/>
+      <c r="C139" s="19"/>
+      <c r="G139" s="21"/>
+    </row>
+    <row r="140" spans="1:7" s="20" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="19"/>
       <c r="B140" s="2"/>
-      <c r="C140" s="21"/>
-      <c r="G140" s="23"/>
-    </row>
-    <row r="141" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A141" s="21"/>
+      <c r="C140" s="19"/>
+      <c r="G140" s="21"/>
+    </row>
+    <row r="141" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A141" s="19"/>
       <c r="B141" s="2"/>
-      <c r="C141" s="21"/>
-      <c r="G141" s="23"/>
-    </row>
-    <row r="142" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A142" s="21"/>
+      <c r="C141" s="19"/>
+      <c r="G141" s="21"/>
+    </row>
+    <row r="142" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A142" s="19"/>
       <c r="B142" s="2"/>
-      <c r="C142" s="21"/>
+      <c r="C142" s="19"/>
       <c r="F142" s="2"/>
-      <c r="G142" s="21"/>
-    </row>
-    <row r="143" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G142" s="19"/>
+    </row>
+    <row r="143" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="4"/>
       <c r="C143" s="6"/>
       <c r="F143" s="2"/>
-      <c r="G143" s="21"/>
-    </row>
-    <row r="144" spans="1:7" s="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G143" s="19"/>
+    </row>
+    <row r="144" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="4"/>
       <c r="C144" s="6"/>
       <c r="F144" s="2"/>
-      <c r="G144" s="21"/>
+      <c r="G144" s="19"/>
     </row>
     <row r="409" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B409" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="I3:I158">
-    <sortCondition ref="I2"/>
+  <sortState ref="A3:C135">
+    <sortCondition ref="A4"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
@@ -4238,783 +4363,783 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>362</v>
+      <c r="A1" s="20" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>390</v>
+      <c r="A3" s="20" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>403</v>
+      <c r="A6" s="20" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>404</v>
+      <c r="A7" s="20" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>401</v>
+      <c r="A8" s="20" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
-        <v>402</v>
+      <c r="A9" s="20" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>368</v>
+      <c r="A10" s="20" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>381</v>
+      <c r="A13" s="20" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>361</v>
+      <c r="A16" s="20" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
-        <v>388</v>
+      <c r="A28" s="20" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>383</v>
+      <c r="A30" s="20" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
-        <v>377</v>
+      <c r="A34" s="20" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
-        <v>376</v>
+      <c r="A36" s="20" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
-        <v>357</v>
+      <c r="A37" s="20" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
-        <v>365</v>
+      <c r="A39" s="20" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="22" t="s">
-        <v>407</v>
-      </c>
-    </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="20" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="22" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="22" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="22" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
         <v>422</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="22" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22" t="s">
-        <v>408</v>
+      <c r="A56" s="20" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="20" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="22" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="20" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="22" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="20" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="22" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="20" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="22" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="22" t="s">
-        <v>415</v>
-      </c>
-    </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="22" t="s">
-        <v>406</v>
+      <c r="A73" s="20" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="22" t="s">
-        <v>369</v>
+      <c r="A74" s="20" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
-        <v>385</v>
+      <c r="A80" s="20" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="22" t="s">
-        <v>374</v>
+      <c r="A81" s="20" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="22" t="s">
-        <v>373</v>
+      <c r="A82" s="20" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="22" t="s">
-        <v>378</v>
+      <c r="A84" s="20" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="22" t="s">
-        <v>366</v>
+      <c r="A94" s="20" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="22" t="s">
-        <v>380</v>
+      <c r="A96" s="20" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="22" t="s">
-        <v>358</v>
+      <c r="A97" s="20" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="22" t="s">
-        <v>386</v>
+      <c r="A99" s="20" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="22" t="s">
+      <c r="A101" s="20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="20" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="22" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="20" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="20" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="22" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="20" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="22" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="20" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="22" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="20" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="22" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="22" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="22" t="s">
-        <v>392</v>
+      <c r="A111" s="20" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="22" t="s">
-        <v>387</v>
+      <c r="A114" s="20" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="22" t="s">
-        <v>384</v>
+      <c r="A116" s="20" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="22" t="s">
-        <v>379</v>
+      <c r="A120" s="20" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="22" t="s">
-        <v>370</v>
+      <c r="A121" s="20" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="22" t="s">
-        <v>375</v>
+      <c r="A125" s="20" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="22" t="s">
-        <v>389</v>
+      <c r="A126" s="20" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="22" t="s">
-        <v>372</v>
+      <c r="A130" s="20" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="22" t="s">
-        <v>367</v>
+      <c r="A139" s="20" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="22" t="s">
-        <v>371</v>
+      <c r="A140" s="20" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="22" t="s">
-        <v>360</v>
+      <c r="A143" s="20" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="22" t="s">
-        <v>363</v>
+      <c r="A148" s="20" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="22" t="s">
-        <v>382</v>
+      <c r="A151" s="20" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="22" t="s">
-        <v>391</v>
+      <c r="A152" s="20" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="22" t="s">
-        <v>359</v>
+      <c r="A155" s="20" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="22" t="s">
-        <v>364</v>
+      <c r="A156" s="20" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>